<commit_message>
Versión 1.0.1 - Corrección error punto de venta
</commit_message>
<xml_diff>
--- a/listado_facturas.xlsx
+++ b/listado_facturas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\bot_facturacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFCA2A8-E5FE-4B2E-A02C-28930B20E0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AD5F87-3FE1-4380-B2CE-AAF355C1F42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{764A6F3F-D110-4813-A95A-0CAE687FCC35}"/>
   </bookViews>
@@ -190,14 +190,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -547,7 +544,7 @@
     <col min="9" max="9" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.42578125" customWidth="1"/>
     <col min="11" max="11" width="29.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="8"/>
+    <col min="13" max="13" width="11.42578125" style="7"/>
     <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="16.85546875" customWidth="1"/>
@@ -555,43 +552,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -608,7 +605,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="9"/>
+      <c r="M2" s="8"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -623,7 +620,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="9"/>
+      <c r="M3" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -637,7 +634,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="9"/>
+      <c r="M4" s="8"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -652,7 +649,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="9"/>
+      <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -667,7 +664,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="9"/>
+      <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -682,7 +679,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="9"/>
+      <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -697,7 +694,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="9"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -712,7 +709,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="9"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -722,12 +719,12 @@
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="4"/>
+      <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="9"/>
+      <c r="M10" s="8"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -742,7 +739,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="9"/>
+      <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -757,7 +754,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="9"/>
+      <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -772,7 +769,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="9"/>
+      <c r="M13" s="8"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -787,7 +784,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="9"/>
+      <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -802,7 +799,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="9"/>
+      <c r="M15" s="8"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -817,7 +814,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
-      <c r="M16" s="9"/>
+      <c r="M16" s="8"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -832,7 +829,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-      <c r="M17" s="9"/>
+      <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
@@ -847,7 +844,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-      <c r="M18" s="9"/>
+      <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
@@ -862,7 +859,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="9"/>
+      <c r="M19" s="8"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -877,7 +874,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="9"/>
+      <c r="M20" s="8"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
@@ -892,7 +889,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="9"/>
+      <c r="M21" s="8"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -907,7 +904,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-      <c r="M22" s="9"/>
+      <c r="M22" s="8"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
@@ -922,7 +919,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-      <c r="M23" s="9"/>
+      <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
@@ -937,7 +934,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-      <c r="M24" s="9"/>
+      <c r="M24" s="8"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -952,7 +949,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
-      <c r="M25" s="9"/>
+      <c r="M25" s="8"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
@@ -967,7 +964,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="9"/>
+      <c r="M26" s="8"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
@@ -982,7 +979,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="9"/>
+      <c r="M27" s="8"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
@@ -997,7 +994,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="9"/>
+      <c r="M28" s="8"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
@@ -1012,7 +1009,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-      <c r="M29" s="9"/>
+      <c r="M29" s="8"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
@@ -1027,7 +1024,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="9"/>
+      <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
@@ -1042,7 +1039,7 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
-      <c r="M31" s="9"/>
+      <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
@@ -1057,7 +1054,7 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-      <c r="M32" s="9"/>
+      <c r="M32" s="8"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
@@ -1072,7 +1069,7 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-      <c r="M33" s="9"/>
+      <c r="M33" s="8"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
@@ -1087,7 +1084,7 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
-      <c r="M34" s="9"/>
+      <c r="M34" s="8"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
@@ -1102,7 +1099,7 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
-      <c r="M35" s="9"/>
+      <c r="M35" s="8"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
@@ -1117,7 +1114,7 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
-      <c r="M36" s="9"/>
+      <c r="M36" s="8"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
@@ -1132,7 +1129,7 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
-      <c r="M37" s="9"/>
+      <c r="M37" s="8"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
@@ -1147,7 +1144,7 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
-      <c r="M38" s="9"/>
+      <c r="M38" s="8"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
@@ -1162,7 +1159,7 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
-      <c r="M39" s="9"/>
+      <c r="M39" s="8"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
@@ -1177,7 +1174,7 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
-      <c r="M40" s="9"/>
+      <c r="M40" s="8"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
@@ -1192,7 +1189,7 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
-      <c r="M41" s="9"/>
+      <c r="M41" s="8"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
@@ -1207,7 +1204,7 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
-      <c r="M42" s="9"/>
+      <c r="M42" s="8"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
@@ -1222,7 +1219,7 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
-      <c r="M43" s="9"/>
+      <c r="M43" s="8"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
@@ -1237,7 +1234,7 @@
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
-      <c r="M44" s="9"/>
+      <c r="M44" s="8"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
@@ -1252,7 +1249,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
-      <c r="M45" s="9"/>
+      <c r="M45" s="8"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
@@ -1267,7 +1264,7 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
-      <c r="M46" s="9"/>
+      <c r="M46" s="8"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
@@ -1282,7 +1279,7 @@
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
-      <c r="M47" s="9"/>
+      <c r="M47" s="8"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
@@ -1297,7 +1294,7 @@
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
-      <c r="M48" s="9"/>
+      <c r="M48" s="8"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
@@ -1312,7 +1309,7 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
-      <c r="M49" s="9"/>
+      <c r="M49" s="8"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
@@ -1327,7 +1324,7 @@
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
-      <c r="M50" s="9"/>
+      <c r="M50" s="8"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
@@ -1342,7 +1339,7 @@
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
-      <c r="M51" s="9"/>
+      <c r="M51" s="8"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
@@ -1357,7 +1354,7 @@
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
-      <c r="M52" s="9"/>
+      <c r="M52" s="8"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
@@ -1372,7 +1369,7 @@
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
-      <c r="M53" s="9"/>
+      <c r="M53" s="8"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
@@ -1387,7 +1384,7 @@
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
-      <c r="M54" s="9"/>
+      <c r="M54" s="8"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
@@ -1402,7 +1399,7 @@
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
-      <c r="M55" s="9"/>
+      <c r="M55" s="8"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
@@ -1417,7 +1414,7 @@
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
-      <c r="M56" s="9"/>
+      <c r="M56" s="8"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
@@ -1432,7 +1429,7 @@
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
-      <c r="M57" s="9"/>
+      <c r="M57" s="8"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
@@ -1447,7 +1444,7 @@
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
-      <c r="M58" s="9"/>
+      <c r="M58" s="8"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
@@ -1462,7 +1459,7 @@
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
-      <c r="M59" s="9"/>
+      <c r="M59" s="8"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
@@ -1477,7 +1474,7 @@
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
-      <c r="M60" s="9"/>
+      <c r="M60" s="8"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
@@ -1492,7 +1489,7 @@
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
-      <c r="M61" s="9"/>
+      <c r="M61" s="8"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
@@ -1507,7 +1504,7 @@
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
-      <c r="M62" s="9"/>
+      <c r="M62" s="8"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
@@ -1522,7 +1519,7 @@
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
-      <c r="M63" s="9"/>
+      <c r="M63" s="8"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
@@ -1537,7 +1534,7 @@
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
-      <c r="M64" s="9"/>
+      <c r="M64" s="8"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
@@ -1552,7 +1549,7 @@
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
-      <c r="M65" s="9"/>
+      <c r="M65" s="8"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
@@ -1567,7 +1564,7 @@
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
-      <c r="M66" s="9"/>
+      <c r="M66" s="8"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
@@ -1582,7 +1579,7 @@
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
-      <c r="M67" s="9"/>
+      <c r="M67" s="8"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
@@ -1597,7 +1594,7 @@
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
-      <c r="M68" s="9"/>
+      <c r="M68" s="8"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
@@ -1612,7 +1609,7 @@
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
-      <c r="M69" s="9"/>
+      <c r="M69" s="8"/>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
@@ -1627,7 +1624,7 @@
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
-      <c r="M70" s="9"/>
+      <c r="M70" s="8"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
@@ -1642,7 +1639,7 @@
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
-      <c r="M71" s="9"/>
+      <c r="M71" s="8"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
@@ -1657,7 +1654,7 @@
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
-      <c r="M72" s="9"/>
+      <c r="M72" s="8"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
@@ -1672,7 +1669,7 @@
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
-      <c r="M73" s="9"/>
+      <c r="M73" s="8"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
@@ -1687,7 +1684,7 @@
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
-      <c r="M74" s="9"/>
+      <c r="M74" s="8"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
@@ -1702,7 +1699,7 @@
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
-      <c r="M75" s="9"/>
+      <c r="M75" s="8"/>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
@@ -1717,7 +1714,7 @@
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
-      <c r="M76" s="9"/>
+      <c r="M76" s="8"/>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
@@ -1732,7 +1729,7 @@
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
-      <c r="M77" s="9"/>
+      <c r="M77" s="8"/>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
@@ -1747,7 +1744,7 @@
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
-      <c r="M78" s="9"/>
+      <c r="M78" s="8"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
@@ -1762,7 +1759,7 @@
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
-      <c r="M79" s="9"/>
+      <c r="M79" s="8"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
@@ -1777,7 +1774,7 @@
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
-      <c r="M80" s="9"/>
+      <c r="M80" s="8"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
@@ -1792,7 +1789,7 @@
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
-      <c r="M81" s="9"/>
+      <c r="M81" s="8"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
@@ -1807,7 +1804,7 @@
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
-      <c r="M82" s="9"/>
+      <c r="M82" s="8"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
@@ -1822,7 +1819,7 @@
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
-      <c r="M83" s="9"/>
+      <c r="M83" s="8"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
@@ -1837,7 +1834,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
-      <c r="M84" s="9"/>
+      <c r="M84" s="8"/>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
@@ -1852,7 +1849,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
-      <c r="M85" s="9"/>
+      <c r="M85" s="8"/>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
@@ -1867,7 +1864,7 @@
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
-      <c r="M86" s="9"/>
+      <c r="M86" s="8"/>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
@@ -1882,7 +1879,7 @@
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
-      <c r="M87" s="9"/>
+      <c r="M87" s="8"/>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
@@ -1897,7 +1894,7 @@
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
-      <c r="M88" s="9"/>
+      <c r="M88" s="8"/>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
@@ -1912,7 +1909,7 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
-      <c r="M89" s="9"/>
+      <c r="M89" s="8"/>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
@@ -1927,7 +1924,7 @@
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
-      <c r="M90" s="9"/>
+      <c r="M90" s="8"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
@@ -1942,7 +1939,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
-      <c r="M91" s="9"/>
+      <c r="M91" s="8"/>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
@@ -1957,7 +1954,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
-      <c r="M92" s="9"/>
+      <c r="M92" s="8"/>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
@@ -1972,7 +1969,7 @@
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
-      <c r="M93" s="9"/>
+      <c r="M93" s="8"/>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
@@ -1987,7 +1984,7 @@
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
-      <c r="M94" s="9"/>
+      <c r="M94" s="8"/>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
@@ -2002,7 +1999,7 @@
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
-      <c r="M95" s="9"/>
+      <c r="M95" s="8"/>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
@@ -2017,7 +2014,7 @@
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
-      <c r="M96" s="9"/>
+      <c r="M96" s="8"/>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
@@ -2032,7 +2029,7 @@
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
-      <c r="M97" s="9"/>
+      <c r="M97" s="8"/>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
@@ -2047,7 +2044,7 @@
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
-      <c r="M98" s="9"/>
+      <c r="M98" s="8"/>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
@@ -2062,7 +2059,7 @@
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
-      <c r="M99" s="9"/>
+      <c r="M99" s="8"/>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
@@ -2077,7 +2074,7 @@
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
-      <c r="M100" s="9"/>
+      <c r="M100" s="8"/>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
@@ -2092,7 +2089,7 @@
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
-      <c r="M101" s="9"/>
+      <c r="M101" s="8"/>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
@@ -2107,7 +2104,7 @@
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
-      <c r="M102" s="9"/>
+      <c r="M102" s="8"/>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
@@ -2122,7 +2119,7 @@
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
-      <c r="M103" s="9"/>
+      <c r="M103" s="8"/>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
@@ -2137,7 +2134,7 @@
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
-      <c r="M104" s="9"/>
+      <c r="M104" s="8"/>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
@@ -2152,7 +2149,7 @@
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
-      <c r="M105" s="9"/>
+      <c r="M105" s="8"/>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
@@ -2167,7 +2164,7 @@
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
-      <c r="M106" s="9"/>
+      <c r="M106" s="8"/>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
@@ -2182,7 +2179,7 @@
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
-      <c r="M107" s="9"/>
+      <c r="M107" s="8"/>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
@@ -2197,7 +2194,7 @@
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
-      <c r="M108" s="9"/>
+      <c r="M108" s="8"/>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
@@ -2212,7 +2209,7 @@
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
-      <c r="M109" s="9"/>
+      <c r="M109" s="8"/>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
@@ -2227,7 +2224,7 @@
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
-      <c r="M110" s="9"/>
+      <c r="M110" s="8"/>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
@@ -2242,7 +2239,7 @@
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
-      <c r="M111" s="9"/>
+      <c r="M111" s="8"/>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
@@ -2257,7 +2254,7 @@
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
-      <c r="M112" s="9"/>
+      <c r="M112" s="8"/>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
@@ -2272,7 +2269,7 @@
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
-      <c r="M113" s="9"/>
+      <c r="M113" s="8"/>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
@@ -2287,7 +2284,7 @@
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
-      <c r="M114" s="9"/>
+      <c r="M114" s="8"/>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
@@ -2302,7 +2299,7 @@
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
-      <c r="M115" s="9"/>
+      <c r="M115" s="8"/>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
@@ -2317,7 +2314,7 @@
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
-      <c r="M116" s="9"/>
+      <c r="M116" s="8"/>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
@@ -2332,7 +2329,7 @@
       <c r="J117" s="2"/>
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
-      <c r="M117" s="9"/>
+      <c r="M117" s="8"/>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
@@ -2347,7 +2344,7 @@
       <c r="J118" s="2"/>
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
-      <c r="M118" s="9"/>
+      <c r="M118" s="8"/>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
@@ -2362,7 +2359,7 @@
       <c r="J119" s="2"/>
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
-      <c r="M119" s="9"/>
+      <c r="M119" s="8"/>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
@@ -2377,7 +2374,7 @@
       <c r="J120" s="2"/>
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
-      <c r="M120" s="9"/>
+      <c r="M120" s="8"/>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
@@ -2392,7 +2389,7 @@
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
-      <c r="M121" s="9"/>
+      <c r="M121" s="8"/>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
@@ -2407,7 +2404,7 @@
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
-      <c r="M122" s="9"/>
+      <c r="M122" s="8"/>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
@@ -2422,7 +2419,7 @@
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
-      <c r="M123" s="9"/>
+      <c r="M123" s="8"/>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
@@ -2437,7 +2434,7 @@
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
       <c r="L124" s="2"/>
-      <c r="M124" s="9"/>
+      <c r="M124" s="8"/>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
@@ -2452,7 +2449,7 @@
       <c r="J125" s="2"/>
       <c r="K125" s="2"/>
       <c r="L125" s="2"/>
-      <c r="M125" s="9"/>
+      <c r="M125" s="8"/>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
@@ -2467,7 +2464,7 @@
       <c r="J126" s="2"/>
       <c r="K126" s="2"/>
       <c r="L126" s="2"/>
-      <c r="M126" s="9"/>
+      <c r="M126" s="8"/>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
@@ -2482,7 +2479,7 @@
       <c r="J127" s="2"/>
       <c r="K127" s="2"/>
       <c r="L127" s="2"/>
-      <c r="M127" s="9"/>
+      <c r="M127" s="8"/>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
@@ -2497,7 +2494,7 @@
       <c r="J128" s="2"/>
       <c r="K128" s="2"/>
       <c r="L128" s="2"/>
-      <c r="M128" s="9"/>
+      <c r="M128" s="8"/>
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
@@ -2512,7 +2509,7 @@
       <c r="J129" s="2"/>
       <c r="K129" s="2"/>
       <c r="L129" s="2"/>
-      <c r="M129" s="9"/>
+      <c r="M129" s="8"/>
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
@@ -2527,7 +2524,7 @@
       <c r="J130" s="2"/>
       <c r="K130" s="2"/>
       <c r="L130" s="2"/>
-      <c r="M130" s="9"/>
+      <c r="M130" s="8"/>
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
@@ -2542,7 +2539,7 @@
       <c r="J131" s="2"/>
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
-      <c r="M131" s="9"/>
+      <c r="M131" s="8"/>
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
@@ -2557,7 +2554,7 @@
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
       <c r="L132" s="2"/>
-      <c r="M132" s="9"/>
+      <c r="M132" s="8"/>
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
@@ -2572,7 +2569,7 @@
       <c r="J133" s="2"/>
       <c r="K133" s="2"/>
       <c r="L133" s="2"/>
-      <c r="M133" s="9"/>
+      <c r="M133" s="8"/>
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
@@ -2587,7 +2584,7 @@
       <c r="J134" s="2"/>
       <c r="K134" s="2"/>
       <c r="L134" s="2"/>
-      <c r="M134" s="9"/>
+      <c r="M134" s="8"/>
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
@@ -2602,7 +2599,7 @@
       <c r="J135" s="2"/>
       <c r="K135" s="2"/>
       <c r="L135" s="2"/>
-      <c r="M135" s="9"/>
+      <c r="M135" s="8"/>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
@@ -2617,16 +2614,16 @@
       <c r="J136" s="2"/>
       <c r="K136" s="2"/>
       <c r="L136" s="2"/>
-      <c r="M136" s="9"/>
+      <c r="M136" s="8"/>
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N139" s="10" t="s">
+      <c r="N139" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="O139" s="10"/>
-      <c r="P139" s="10"/>
-      <c r="Q139" s="10"/>
-      <c r="R139" s="10"/>
+      <c r="O139" s="9"/>
+      <c r="P139" s="9"/>
+      <c r="Q139" s="9"/>
+      <c r="R139" s="9"/>
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N140" t="s">

</xml_diff>

<commit_message>
Se agrega sección créditos, se modifica readme para publicar v1.0
</commit_message>
<xml_diff>
--- a/listado_facturas.xlsx
+++ b/listado_facturas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\bot_facturacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmend\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AD5F87-3FE1-4380-B2CE-AAF355C1F42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C842CED3-E6CF-4829-9EA4-E12B5A9817B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{764A6F3F-D110-4813-A95A-0CAE687FCC35}"/>
   </bookViews>
@@ -152,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -186,11 +186,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -210,7 +241,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -527,7 +564,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D0202D-C865-4310-9D27-DD0FBA868814}">
-  <dimension ref="A1:R143"/>
+  <dimension ref="A1:S136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -545,13 +582,16 @@
     <col min="10" max="10" width="30.42578125" customWidth="1"/>
     <col min="11" max="11" width="29.7109375" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" style="7"/>
-    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" customWidth="1"/>
+    <col min="18" max="18" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.5703125" customWidth="1"/>
     <col min="25" max="26" width="16.85546875" customWidth="1"/>
     <col min="27" max="27" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -591,8 +631,15 @@
       <c r="M1" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="11"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -606,8 +653,23 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="8"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -621,8 +683,23 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="8"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -635,8 +712,19 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="8"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O4" s="2"/>
+      <c r="P4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -650,8 +738,19 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="8"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O5" s="2"/>
+      <c r="P5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -666,7 +765,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="8"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -681,7 +780,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -696,7 +795,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -711,7 +810,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -726,7 +825,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -741,7 +840,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -756,7 +855,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -771,7 +870,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -786,7 +885,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -801,7 +900,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2496,7 +2595,7 @@
       <c r="L128" s="2"/>
       <c r="M128" s="8"/>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -2511,7 +2610,7 @@
       <c r="L129" s="2"/>
       <c r="M129" s="8"/>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -2526,7 +2625,7 @@
       <c r="L130" s="2"/>
       <c r="M130" s="8"/>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -2541,7 +2640,7 @@
       <c r="L131" s="2"/>
       <c r="M131" s="8"/>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -2556,7 +2655,7 @@
       <c r="L132" s="2"/>
       <c r="M132" s="8"/>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
@@ -2571,7 +2670,7 @@
       <c r="L133" s="2"/>
       <c r="M133" s="8"/>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
@@ -2586,7 +2685,7 @@
       <c r="L134" s="2"/>
       <c r="M134" s="8"/>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -2601,7 +2700,7 @@
       <c r="L135" s="2"/>
       <c r="M135" s="8"/>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
@@ -2616,90 +2715,25 @@
       <c r="L136" s="2"/>
       <c r="M136" s="8"/>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N139" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="O139" s="9"/>
-      <c r="P139" s="9"/>
-      <c r="Q139" s="9"/>
-      <c r="R139" s="9"/>
-    </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N140" t="s">
-        <v>6</v>
-      </c>
-      <c r="O140" t="s">
-        <v>9</v>
-      </c>
-      <c r="P140" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q140" t="s">
-        <v>13</v>
-      </c>
-      <c r="R140" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="N141" t="s">
-        <v>5</v>
-      </c>
-      <c r="O141" t="s">
-        <v>10</v>
-      </c>
-      <c r="P141" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q141" t="s">
-        <v>14</v>
-      </c>
-      <c r="R141" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="O142" t="s">
-        <v>11</v>
-      </c>
-      <c r="P142" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q142" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="O143" t="s">
-        <v>12</v>
-      </c>
-      <c r="P143" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q143" t="s">
-        <v>16</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="N139:R139"/>
+    <mergeCell ref="O1:S1"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F136" xr:uid="{9550D9F4-EBAA-4C64-9961-20701D99359B}">
-      <formula1>$Q$140:$Q$143</formula1>
+      <formula1>$R$2:$R$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C136" xr:uid="{C6F88E93-E31A-4676-808F-D514930024C2}">
-      <formula1>$N$140:$N$141</formula1>
+      <formula1>$O$2:$O$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J136" xr:uid="{AF9D46F2-F742-466A-8FCF-0B8844FBC611}">
-      <formula1>$O$140:$O$143</formula1>
+      <formula1>$P$2:$P$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G136" xr:uid="{FB46B816-26D7-4FB4-9A37-D8503938107B}">
-      <formula1>$P$140:$P$143</formula1>
+      <formula1>$Q$2:$Q$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M136" xr:uid="{3FDC47DE-30F1-4FF1-B805-D456249842F0}">
-      <formula1>$R$140:$R$141</formula1>
+      <formula1>$S$2:$S$3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>